<commit_message>
set optimal architecture for sim 3 50
</commit_message>
<xml_diff>
--- a/efficiency_testing/sim_3_50/Optimizer_Testing_NN_outcome.xlsx
+++ b/efficiency_testing/sim_3_50/Optimizer_Testing_NN_outcome.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcg\Google Drive\MasterThesis\dml_est_general\efficiency_testing\sim_2_50\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcg\Google Drive\MasterThesis\dml_est_general\efficiency_testing\sim_3_50\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BE3A13-11BF-4494-8C6C-F8F2BD6C4D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB07A25-FC82-4958-8DCA-9A0D53A2A708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Single_Layer" sheetId="4" r:id="rId1"/>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF281ED2-ABAB-40DD-9295-A7DCC4583589}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,52 +743,52 @@
         <v>0.01</v>
       </c>
       <c r="C7" s="1">
-        <v>5.09</v>
+        <v>8.08</v>
       </c>
       <c r="D7" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="E7" s="1">
-        <v>4.7699999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="F7" s="1">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="G7" s="1">
-        <v>3.84</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="H7" s="1">
-        <v>1.22</v>
+        <v>1.26</v>
       </c>
       <c r="I7" s="1">
-        <v>3.79</v>
+        <v>4.07</v>
       </c>
       <c r="J7" s="1">
-        <v>1.24</v>
+        <v>1.28</v>
       </c>
       <c r="K7" s="1">
-        <v>6.83</v>
+        <v>8.48</v>
       </c>
       <c r="L7" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="M7" s="1">
-        <v>6.57</v>
+        <v>7.19</v>
       </c>
       <c r="N7" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="O7" s="1">
-        <v>6.23</v>
+        <v>7.11</v>
       </c>
       <c r="P7" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="Q7" s="1">
-        <v>6.55</v>
+        <v>7.52</v>
       </c>
       <c r="R7" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -799,52 +799,52 @@
         <v>0.01</v>
       </c>
       <c r="C8" s="1">
-        <v>9.11</v>
+        <v>12.64</v>
       </c>
       <c r="D8" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="E8" s="1">
-        <v>6.64</v>
+        <v>10.17</v>
       </c>
       <c r="F8" s="1">
-        <v>1.17</v>
+        <v>1.24</v>
       </c>
       <c r="G8" s="1">
-        <v>5.64</v>
+        <v>6.16</v>
       </c>
       <c r="H8" s="1">
-        <v>1.18</v>
+        <v>1.24</v>
       </c>
       <c r="I8" s="1">
-        <v>5.1100000000000003</v>
+        <v>5.31</v>
       </c>
       <c r="J8" s="1">
-        <v>1.19</v>
+        <v>1.25</v>
       </c>
       <c r="K8" s="1">
-        <v>14.67</v>
+        <v>16.77</v>
       </c>
       <c r="L8" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="M8" s="1">
-        <v>11.7</v>
+        <v>16.18</v>
       </c>
       <c r="N8" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="O8" s="1">
-        <v>12.09</v>
+        <v>13.78</v>
       </c>
       <c r="P8" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="Q8" s="1">
-        <v>12.04</v>
+        <v>12.24</v>
       </c>
       <c r="R8" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -855,52 +855,52 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="1">
-        <v>5.87</v>
+        <v>9.32</v>
       </c>
       <c r="D9" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="E9" s="1">
-        <v>5.05</v>
+        <v>8.26</v>
       </c>
       <c r="F9" s="1">
-        <v>1.18</v>
+        <v>1.22</v>
       </c>
       <c r="G9" s="1">
-        <v>4.5599999999999996</v>
+        <v>5.93</v>
       </c>
       <c r="H9" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1.2</v>
+        <v>1.23</v>
+      </c>
+      <c r="I9" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="J9" s="7">
+        <v>1.22</v>
       </c>
       <c r="K9" s="1">
-        <v>10.17</v>
+        <v>15.07</v>
       </c>
       <c r="L9" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="M9" s="1">
-        <v>11.3</v>
+        <v>13.33</v>
       </c>
       <c r="N9" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="O9" s="1">
-        <v>12.08</v>
+        <v>14.9</v>
       </c>
       <c r="P9" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="Q9" s="1">
-        <v>14.58</v>
+        <v>14.81</v>
       </c>
       <c r="R9" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -911,52 +911,52 @@
         <v>0.01</v>
       </c>
       <c r="C10" s="1">
-        <v>5.65</v>
+        <v>6.08</v>
       </c>
       <c r="D10" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="E10" s="1">
-        <v>5.04</v>
+        <v>7.34</v>
       </c>
       <c r="F10" s="1">
-        <v>1.2</v>
+        <v>1.24</v>
       </c>
       <c r="G10" s="1">
-        <v>4.6399999999999997</v>
+        <v>5.26</v>
       </c>
       <c r="H10" s="1">
-        <v>1.22</v>
+        <v>1.27</v>
       </c>
       <c r="I10" s="1">
-        <v>4.0999999999999996</v>
+        <v>5.88</v>
       </c>
       <c r="J10" s="1">
-        <v>1.24</v>
+        <v>1.28</v>
       </c>
       <c r="K10" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="M10" s="1">
+        <v>8.02</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="O10" s="1">
         <v>7.93</v>
       </c>
-      <c r="L10" s="1">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M10" s="1">
-        <v>6.71</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="O10" s="1">
-        <v>6.55</v>
-      </c>
       <c r="P10" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="Q10" s="1">
-        <v>6.89</v>
+        <v>8.39</v>
       </c>
       <c r="R10" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -967,52 +967,52 @@
         <v>0.01</v>
       </c>
       <c r="C11" s="1">
-        <v>22.47</v>
+        <v>23.91</v>
       </c>
       <c r="D11" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="E11" s="1">
-        <v>19.170000000000002</v>
+        <v>23.23</v>
       </c>
       <c r="F11" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="G11" s="1">
-        <v>23.03</v>
+        <v>17.739999999999998</v>
       </c>
       <c r="H11" s="1">
-        <v>1.17</v>
+        <v>1.25</v>
       </c>
       <c r="I11" s="1">
-        <v>14.89</v>
+        <v>18.440000000000001</v>
       </c>
       <c r="J11" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="K11" s="1">
-        <v>29.56</v>
+        <v>26.5</v>
       </c>
       <c r="L11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.37</v>
       </c>
       <c r="M11" s="1">
-        <v>29.53</v>
+        <v>15.72</v>
       </c>
       <c r="N11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.37</v>
       </c>
       <c r="O11" s="1">
-        <v>22.73</v>
+        <v>9.19</v>
       </c>
       <c r="P11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.38</v>
       </c>
       <c r="Q11" s="1">
-        <v>19.93</v>
+        <v>7.7</v>
       </c>
       <c r="R11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1021,35 +1021,35 @@
       </c>
       <c r="D13">
         <f>MIN(D7:D11)</f>
-        <v>1.1499999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="F13">
         <f>MIN(F7:F11)</f>
-        <v>1.1499999999999999</v>
+        <v>1.22</v>
       </c>
       <c r="H13">
         <f>MIN(H7:H11)</f>
-        <v>1.17</v>
+        <v>1.23</v>
       </c>
       <c r="J13">
         <f>MIN(J7:J11)</f>
-        <v>1.1599999999999999</v>
+        <v>1.22</v>
       </c>
       <c r="L13">
         <f>MIN(L7:L11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.29</v>
       </c>
       <c r="N13">
         <f>MIN(N7:N11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.29</v>
       </c>
       <c r="P13">
         <f>MIN(P7:P11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.29</v>
       </c>
       <c r="R13">
         <f>MIN(R7:R11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
-        <v>1.1200000000000001</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1069,33 +1069,33 @@
         <f>IF(_xlfn.MINIFS(C7:C11,D7:D11,$D$14) = 0, NA(), _xlfn.MINIFS(C7:C11,D7:D11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" t="e">
+      <c r="F15">
         <f>IF(_xlfn.MINIFS(E7:E11,F7:F11,$D$14) = 0, NA(), _xlfn.MINIFS(E7:E11,F7:F11,$D$14))</f>
-        <v>#N/A</v>
+        <v>8.26</v>
       </c>
       <c r="H15" t="e">
         <f>IF(_xlfn.MINIFS(G7:G11,H7:H11,$D$14) = 0, NA(), _xlfn.MINIFS(G7:G11,H7:H11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="J15" t="e">
+      <c r="J15">
         <f>IF(_xlfn.MINIFS(I7:I11,J7:J11,$D$14) = 0, NA(), _xlfn.MINIFS(I7:I11,J7:J11,$D$14))</f>
+        <v>5.7</v>
+      </c>
+      <c r="L15" t="e">
+        <f>IF(_xlfn.MINIFS(K7:K11,L7:L11,$D$14) = 0, NA(), _xlfn.MINIFS(K7:K11,L7:L11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="L15">
-        <f>IF(_xlfn.MINIFS(K7:K11,L7:L11,$D$14) = 0, NA(), _xlfn.MINIFS(K7:K11,L7:L11,$D$14))</f>
-        <v>29.56</v>
-      </c>
-      <c r="N15">
+      <c r="N15" t="e">
         <f>IF(_xlfn.MINIFS(M7:M11,N7:N11,$D$14) = 0, NA(), _xlfn.MINIFS(M7:M11,N7:N11,$D$14))</f>
-        <v>29.53</v>
-      </c>
-      <c r="P15">
+        <v>#N/A</v>
+      </c>
+      <c r="P15" t="e">
         <f>IF(_xlfn.MINIFS(O7:O11,P7:P11,$D$14) = 0, NA(), _xlfn.MINIFS(O7:O11,P7:P11,$D$14))</f>
-        <v>22.73</v>
-      </c>
-      <c r="R15">
+        <v>#N/A</v>
+      </c>
+      <c r="R15" t="e">
         <f>IF(_xlfn.MINIFS(Q7:Q11,R7:R11,$D$14) = 0, NA(), _xlfn.MINIFS(Q7:Q11,R7:R11,$D$14))</f>
-        <v>19.93</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="D16">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
-        <v>19.93</v>
+        <v>5.7</v>
       </c>
     </row>
   </sheetData>
@@ -1146,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7163045-D3C2-43D0-B4A2-2C5E78C3DE32}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1340,52 +1340,52 @@
         <v>0.01</v>
       </c>
       <c r="C7" s="1">
-        <v>5.07</v>
+        <v>5.82</v>
       </c>
       <c r="D7" s="1">
-        <v>1.18</v>
+        <v>1.27</v>
       </c>
       <c r="E7" s="1">
-        <v>4.1900000000000004</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F7" s="1">
-        <v>1.23</v>
+        <v>1.29</v>
       </c>
       <c r="G7" s="1">
-        <v>4.79</v>
+        <v>5.24</v>
       </c>
       <c r="H7" s="1">
-        <v>1.2</v>
+        <v>1.28</v>
       </c>
       <c r="I7" s="1">
-        <v>3.88</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="J7" s="1">
-        <v>1.24</v>
+        <v>1.29</v>
       </c>
       <c r="K7" s="1">
-        <v>6.31</v>
+        <v>7.41</v>
       </c>
       <c r="L7" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="M7" s="1">
-        <v>5.61</v>
+        <v>6.62</v>
       </c>
       <c r="N7" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="O7" s="1">
-        <v>5.76</v>
+        <v>7.23</v>
       </c>
       <c r="P7" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="Q7" s="1">
-        <v>5.33</v>
+        <v>6.9</v>
       </c>
       <c r="R7" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1396,52 +1396,52 @@
         <v>0.01</v>
       </c>
       <c r="C8" s="1">
-        <v>8.61</v>
+        <v>10.42</v>
       </c>
       <c r="D8" s="1">
-        <v>1.17</v>
+        <v>1.26</v>
       </c>
       <c r="E8" s="1">
-        <v>5.82</v>
+        <v>6.46</v>
       </c>
       <c r="F8" s="1">
-        <v>1.2</v>
+        <v>1.26</v>
       </c>
       <c r="G8" s="1">
-        <v>7.14</v>
+        <v>7.16</v>
       </c>
       <c r="H8" s="1">
-        <v>1.18</v>
+        <v>1.27</v>
       </c>
       <c r="I8" s="1">
-        <v>5.98</v>
+        <v>6.73</v>
       </c>
       <c r="J8" s="1">
-        <v>1.2</v>
+        <v>1.26</v>
       </c>
       <c r="K8" s="1">
-        <v>12.2</v>
+        <v>11</v>
       </c>
       <c r="L8" s="1">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M8" s="7">
-        <v>9.74</v>
-      </c>
-      <c r="N8" s="7">
-        <v>1.1200000000000001</v>
+        <v>1.28</v>
+      </c>
+      <c r="M8" s="1">
+        <v>13.97</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1.27</v>
       </c>
       <c r="O8" s="1">
-        <v>10.78</v>
+        <v>12.68</v>
       </c>
       <c r="P8" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="Q8" s="1">
-        <v>9.4600000000000009</v>
+        <v>11.56</v>
       </c>
       <c r="R8" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1452,52 +1452,52 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="1">
-        <v>4.76</v>
+        <v>5.71</v>
       </c>
       <c r="D9" s="1">
-        <v>1.17</v>
+        <v>1.23</v>
       </c>
       <c r="E9" s="1">
-        <v>5.0999999999999996</v>
+        <v>4.82</v>
       </c>
       <c r="F9" s="1">
-        <v>1.2</v>
+        <v>1.26</v>
       </c>
       <c r="G9" s="1">
-        <v>5.16</v>
+        <v>5.23</v>
       </c>
       <c r="H9" s="1">
-        <v>1.18</v>
+        <v>1.26</v>
       </c>
       <c r="I9" s="1">
-        <v>4.9800000000000004</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="J9" s="1">
-        <v>1.21</v>
+        <v>1.27</v>
       </c>
       <c r="K9" s="1">
-        <v>9.27</v>
+        <v>13.12</v>
       </c>
       <c r="L9" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="M9" s="1">
-        <v>8.15</v>
+        <v>13.82</v>
       </c>
       <c r="N9" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="O9" s="1">
-        <v>10.6</v>
+        <v>12.74</v>
       </c>
       <c r="P9" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="Q9" s="1">
-        <v>7.93</v>
+        <v>11.12</v>
       </c>
       <c r="R9" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1508,52 +1508,52 @@
         <v>0.01</v>
       </c>
       <c r="C10" s="1">
-        <v>5.89</v>
+        <v>5.34</v>
       </c>
       <c r="D10" s="1">
-        <v>1.19</v>
+        <v>1.29</v>
       </c>
       <c r="E10" s="1">
-        <v>4.72</v>
+        <v>4.99</v>
       </c>
       <c r="F10" s="1">
-        <v>1.24</v>
+        <v>1.28</v>
       </c>
       <c r="G10" s="1">
-        <v>6.11</v>
+        <v>5.71</v>
       </c>
       <c r="H10" s="1">
-        <v>1.2</v>
+        <v>1.27</v>
       </c>
       <c r="I10" s="1">
-        <v>4.5599999999999996</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="J10" s="1">
-        <v>1.24</v>
+        <v>1.3</v>
       </c>
       <c r="K10" s="1">
-        <v>7.56</v>
+        <v>8.09</v>
       </c>
       <c r="L10" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="M10" s="1">
-        <v>7.99</v>
+        <v>7.72</v>
       </c>
       <c r="N10" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="O10" s="1">
-        <v>7.01</v>
+        <v>7.67</v>
       </c>
       <c r="P10" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="Q10" s="1">
-        <v>6.09</v>
+        <v>7.52</v>
       </c>
       <c r="R10" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1564,52 +1564,52 @@
         <v>0.01</v>
       </c>
       <c r="C11" s="1">
-        <v>18.14</v>
+        <v>24.02</v>
       </c>
       <c r="D11" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="E11" s="1">
-        <v>17.52</v>
+        <v>17.8</v>
       </c>
       <c r="F11" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="G11" s="1">
-        <v>19.579999999999998</v>
+        <v>21.72</v>
       </c>
       <c r="H11" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="I11" s="1">
-        <v>15.14</v>
+        <v>21.29</v>
       </c>
       <c r="J11" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="K11" s="1">
-        <v>28.49</v>
+        <v>27.62</v>
       </c>
       <c r="L11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.34</v>
       </c>
       <c r="M11" s="1">
-        <v>21.59</v>
+        <v>20.6</v>
       </c>
       <c r="N11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.33</v>
       </c>
       <c r="O11" s="1">
-        <v>23.59</v>
+        <v>25.47</v>
       </c>
       <c r="P11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.33</v>
       </c>
       <c r="Q11" s="1">
-        <v>22.33</v>
+        <v>25.17</v>
       </c>
       <c r="R11" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1618,35 +1618,35 @@
       </c>
       <c r="D13">
         <f>MIN(D8:D11)</f>
-        <v>1.1499999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="F13">
         <f>MIN(F8:F11)</f>
-        <v>1.1599999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="H13">
         <f>MIN(H8:H11)</f>
-        <v>1.1499999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="J13">
         <f>MIN(J8:J11)</f>
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="L13">
         <f>MIN(L8:L11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.28</v>
       </c>
       <c r="N13">
         <f>MIN(N8:N11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="P13">
         <f>MIN(P8:P11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="R13">
         <f>MIN(R8:R11)</f>
-        <v>1.1200000000000001</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1655,16 +1655,16 @@
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
-        <v>1.1200000000000001</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="e">
+      <c r="D15">
         <f>IF(_xlfn.MINIFS(C8:C11,D8:D11,$D$14) = 0, NA(), _xlfn.MINIFS(C8:C11,D8:D11,$D$14))</f>
-        <v>#N/A</v>
+        <v>5.71</v>
       </c>
       <c r="F15" t="e">
         <f>IF(_xlfn.MINIFS(E8:E11,F8:F11,$D$14) = 0, NA(), _xlfn.MINIFS(E8:E11,F8:F11,$D$14))</f>
@@ -1678,21 +1678,21 @@
         <f>IF(_xlfn.MINIFS(I8:I11,J8:J11,$D$14) = 0, NA(), _xlfn.MINIFS(I8:I11,J8:J11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="L15">
+      <c r="L15" t="e">
         <f>IF(_xlfn.MINIFS(K8:K11,L8:L11,$D$14) = 0, NA(), _xlfn.MINIFS(K8:K11,L8:L11,$D$14))</f>
-        <v>28.49</v>
-      </c>
-      <c r="N15">
+        <v>#N/A</v>
+      </c>
+      <c r="N15" t="e">
         <f>IF(_xlfn.MINIFS(M8:M11,N8:N11,$D$14) = 0, NA(), _xlfn.MINIFS(M8:M11,N8:N11,$D$14))</f>
-        <v>9.74</v>
-      </c>
-      <c r="P15">
+        <v>#N/A</v>
+      </c>
+      <c r="P15" t="e">
         <f>IF(_xlfn.MINIFS(O8:O11,P8:P11,$D$14) = 0, NA(), _xlfn.MINIFS(O8:O11,P8:P11,$D$14))</f>
-        <v>23.59</v>
-      </c>
-      <c r="R15">
+        <v>#N/A</v>
+      </c>
+      <c r="R15" t="e">
         <f>IF(_xlfn.MINIFS(Q8:Q11,R8:R11,$D$14) = 0, NA(), _xlfn.MINIFS(Q8:Q11,R8:R11,$D$14))</f>
-        <v>22.33</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="D16">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
-        <v>9.74</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -1882,52 +1882,52 @@
         <v>0.01</v>
       </c>
       <c r="C22" s="1">
-        <v>5.43</v>
+        <v>7.2</v>
       </c>
       <c r="D22" s="1">
-        <v>1.17</v>
+        <v>1.26</v>
       </c>
       <c r="E22" s="1">
-        <v>4.99</v>
+        <v>5.96</v>
       </c>
       <c r="F22" s="1">
-        <v>1.2</v>
+        <v>1.27</v>
       </c>
       <c r="G22" s="1">
-        <v>4.97</v>
+        <v>6.45</v>
       </c>
       <c r="H22" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="I22" s="1">
-        <v>4.68</v>
+        <v>5.72</v>
       </c>
       <c r="J22" s="1">
-        <v>1.19</v>
+        <v>1.27</v>
       </c>
       <c r="K22" s="1">
-        <v>7.86</v>
+        <v>8.07</v>
       </c>
       <c r="L22" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="M22" s="1">
-        <v>7.59</v>
+        <v>6.84</v>
       </c>
       <c r="N22" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="O22" s="1">
-        <v>7.29</v>
+        <v>8.01</v>
       </c>
       <c r="P22" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="Q22" s="1">
-        <v>7.25</v>
+        <v>6.92</v>
       </c>
       <c r="R22" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -1938,52 +1938,52 @@
         <v>0.01</v>
       </c>
       <c r="C23" s="1">
-        <v>7.8</v>
+        <v>15.84</v>
       </c>
       <c r="D23" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="E23" s="1">
-        <v>7.21</v>
+        <v>9.85</v>
       </c>
       <c r="F23" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="G23" s="1">
-        <v>8.82</v>
+        <v>8.92</v>
       </c>
       <c r="H23" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="I23" s="1">
-        <v>6.54</v>
+        <v>8.57</v>
       </c>
       <c r="J23" s="1">
-        <v>1.17</v>
+        <v>1.26</v>
       </c>
       <c r="K23" s="1">
-        <v>15.74</v>
+        <v>15.56</v>
       </c>
       <c r="L23" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="M23" s="1">
-        <v>12.49</v>
+        <v>15.59</v>
       </c>
       <c r="N23" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="O23" s="1">
-        <v>14.88</v>
+        <v>13.9</v>
       </c>
       <c r="P23" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="Q23" s="1">
-        <v>12.44</v>
+        <v>14.44</v>
       </c>
       <c r="R23" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -1994,52 +1994,52 @@
         <v>0.1</v>
       </c>
       <c r="C24" s="1">
-        <v>6.72</v>
+        <v>7.71</v>
       </c>
       <c r="D24" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="E24" s="1">
-        <v>5.16</v>
+        <v>8.48</v>
       </c>
       <c r="F24" s="1">
-        <v>1.17</v>
+        <v>1.26</v>
       </c>
       <c r="G24" s="1">
-        <v>6.79</v>
+        <v>6.83</v>
       </c>
       <c r="H24" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="I24" s="1">
-        <v>4.67</v>
+        <v>7.93</v>
       </c>
       <c r="J24" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="K24" s="1">
-        <v>15.01</v>
+        <v>16.440000000000001</v>
       </c>
       <c r="L24" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="M24" s="1">
-        <v>13.96</v>
+        <v>18.059999999999999</v>
       </c>
       <c r="N24" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="O24" s="1">
-        <v>11.75</v>
+        <v>15.25</v>
       </c>
       <c r="P24" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="Q24" s="1">
-        <v>15.13</v>
+        <v>14.64</v>
       </c>
       <c r="R24" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -2050,52 +2050,52 @@
         <v>0.01</v>
       </c>
       <c r="C25" s="1">
-        <v>6.27</v>
+        <v>5.97</v>
       </c>
       <c r="D25" s="1">
-        <v>1.17</v>
+        <v>1.29</v>
       </c>
       <c r="E25" s="1">
-        <v>4.82</v>
+        <v>6.65</v>
       </c>
       <c r="F25" s="1">
-        <v>1.18</v>
+        <v>1.26</v>
       </c>
       <c r="G25" s="1">
-        <v>5.43</v>
+        <v>7.27</v>
       </c>
       <c r="H25" s="1">
-        <v>1.17</v>
+        <v>1.26</v>
       </c>
       <c r="I25" s="1">
-        <v>4.9400000000000004</v>
+        <v>5.58</v>
       </c>
       <c r="J25" s="1">
-        <v>1.19</v>
+        <v>1.28</v>
       </c>
       <c r="K25" s="1">
-        <v>7.55</v>
+        <v>9.66</v>
       </c>
       <c r="L25" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="M25" s="1">
-        <v>7.59</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="N25" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="O25" s="1">
-        <v>7.94</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="P25" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="Q25" s="1">
-        <v>7.1</v>
+        <v>8.6</v>
       </c>
       <c r="R25" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -2106,52 +2106,52 @@
         <v>0.01</v>
       </c>
       <c r="C26" s="1">
-        <v>29.44</v>
+        <v>29.61</v>
       </c>
       <c r="D26" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="E26" s="1">
-        <v>25.9</v>
+        <v>30.4</v>
       </c>
       <c r="F26" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="G26" s="1">
-        <v>26.2</v>
+        <v>30.76</v>
       </c>
       <c r="H26" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="I26" s="1">
-        <v>25.3</v>
+        <v>29.49</v>
       </c>
       <c r="J26" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="K26" s="1">
-        <v>31.26</v>
+        <v>29.87</v>
       </c>
       <c r="L26" s="1">
-        <v>1.17</v>
+        <v>1.39</v>
       </c>
       <c r="M26" s="1">
-        <v>29.93</v>
+        <v>26.67</v>
       </c>
       <c r="N26" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.38</v>
       </c>
       <c r="O26" s="1">
-        <v>31.19</v>
+        <v>24.95</v>
       </c>
       <c r="P26" s="1">
-        <v>1.17</v>
+        <v>1.39</v>
       </c>
       <c r="Q26" s="1">
-        <v>31.41</v>
+        <v>23.77</v>
       </c>
       <c r="R26" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -2160,35 +2160,35 @@
       </c>
       <c r="D28">
         <f>MIN(D22:D26)</f>
-        <v>1.1399999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28" si="0">MIN(F22:F26)</f>
-        <v>1.1499999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="H28">
         <f t="shared" ref="H28" si="1">MIN(H22:H26)</f>
-        <v>1.1299999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="J28">
         <f t="shared" ref="J28" si="2">MIN(J22:J26)</f>
-        <v>1.1399999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="L28">
         <f t="shared" ref="L28" si="3">MIN(L22:L26)</f>
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="N28">
         <f t="shared" ref="N28" si="4">MIN(N22:N26)</f>
-        <v>1.1299999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="P28">
         <f t="shared" ref="P28" si="5">MIN(P22:P26)</f>
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="R28">
         <f t="shared" ref="R28" si="6">MIN(R22:R26)</f>
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2197,43 +2197,43 @@
       </c>
       <c r="D29">
         <f>MIN(D28:R28)</f>
-        <v>1.1299999999999999</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="D30" t="e">
-        <f>IF(_xlfn.MINIFS(C22:C26,D22:D26,$D$14) = 0, NA(), _xlfn.MINIFS(C22:C26,D22:D26,$D$14))</f>
+      <c r="D30">
+        <f>IF(_xlfn.MINIFS(C22:C26,D22:D26,$D$29) = 0, NA(), _xlfn.MINIFS(C22:C26,D22:D26,$D$29))</f>
+        <v>15.84</v>
+      </c>
+      <c r="F30" t="e">
+        <f>IF(_xlfn.MINIFS(E22:E26,F22:F26,$D$29) = 0, NA(), _xlfn.MINIFS(E22:E26,F22:F26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="F30" t="e">
-        <f t="shared" ref="F30" si="7">IF(_xlfn.MINIFS(E22:E26,F22:F26,$D$14) = 0, NA(), _xlfn.MINIFS(E22:E26,F22:F26,$D$14))</f>
+      <c r="H30">
+        <f>IF(_xlfn.MINIFS(G22:G26,H22:H26,$D$29) = 0, NA(), _xlfn.MINIFS(G22:G26,H22:H26,$D$29))</f>
+        <v>6.45</v>
+      </c>
+      <c r="J30" t="e">
+        <f>IF(_xlfn.MINIFS(I22:I26,J22:J26,$D$29) = 0, NA(), _xlfn.MINIFS(I22:I26,J22:J26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="H30" t="e">
-        <f t="shared" ref="H30" si="8">IF(_xlfn.MINIFS(G22:G26,H22:H26,$D$14) = 0, NA(), _xlfn.MINIFS(G22:G26,H22:H26,$D$14))</f>
+      <c r="L30" t="e">
+        <f>IF(_xlfn.MINIFS(K22:K26,L22:L26,$D$29) = 0, NA(), _xlfn.MINIFS(K22:K26,L22:L26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="J30" t="e">
-        <f t="shared" ref="J30" si="9">IF(_xlfn.MINIFS(I22:I26,J22:J26,$D$14) = 0, NA(), _xlfn.MINIFS(I22:I26,J22:J26,$D$14))</f>
+      <c r="N30" t="e">
+        <f>IF(_xlfn.MINIFS(M22:M26,N22:N26,$D$29) = 0, NA(), _xlfn.MINIFS(M22:M26,N22:N26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="L30" t="e">
-        <f t="shared" ref="L30" si="10">IF(_xlfn.MINIFS(K22:K26,L22:L26,$D$14) = 0, NA(), _xlfn.MINIFS(K22:K26,L22:L26,$D$14))</f>
+      <c r="P30" t="e">
+        <f>IF(_xlfn.MINIFS(O22:O26,P22:P26,$D$29) = 0, NA(), _xlfn.MINIFS(O22:O26,P22:P26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="N30" t="e">
-        <f t="shared" ref="N30" si="11">IF(_xlfn.MINIFS(M22:M26,N22:N26,$D$14) = 0, NA(), _xlfn.MINIFS(M22:M26,N22:N26,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P30" t="e">
-        <f t="shared" ref="P30" si="12">IF(_xlfn.MINIFS(O22:O26,P22:P26,$D$14) = 0, NA(), _xlfn.MINIFS(O22:O26,P22:P26,$D$14))</f>
-        <v>#N/A</v>
-      </c>
       <c r="R30" t="e">
-        <f t="shared" ref="R30" si="13">IF(_xlfn.MINIFS(Q22:Q26,R22:R26,$D$14) = 0, NA(), _xlfn.MINIFS(Q22:Q26,R22:R26,$D$14))</f>
+        <f>IF(_xlfn.MINIFS(Q22:Q26,R22:R26,$D$29) = 0, NA(), _xlfn.MINIFS(Q22:Q26,R22:R26,$D$29))</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="D31">
         <f t="array" ref="D31">MIN(IF(ISNUMBER(D30:R30),D30:R30,""))</f>
-        <v>0</v>
+        <v>6.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>